<commit_message>
Modified variable names and stateObjective function
</commit_message>
<xml_diff>
--- a/reflexion IA.xlsx
+++ b/reflexion IA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5088" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="6300" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="58">
   <si>
     <t>algorithme avec 1 détour</t>
   </si>
@@ -149,6 +149,45 @@
   </si>
   <si>
     <t>forceEnd</t>
+  </si>
+  <si>
+    <t>fonctionnement :</t>
+  </si>
+  <si>
+    <t>tout en horizontal, puis tout en vertical</t>
+  </si>
+  <si>
+    <t>retirer tout a partir de l'erreur</t>
+  </si>
+  <si>
+    <t>tous les horizontaux restant</t>
+  </si>
+  <si>
+    <t>tous les verticaux restant</t>
+  </si>
+  <si>
+    <t>un vertical</t>
+  </si>
+  <si>
+    <t>retirer tout a partir du dernier horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remettre toute la partie verticale avant l'erreur </t>
+  </si>
+  <si>
+    <t>deux verticaux</t>
+  </si>
+  <si>
+    <t>pas de solution:</t>
+  </si>
+  <si>
+    <t>arret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erreur en horizontal + un vertical dispo : </t>
+  </si>
+  <si>
+    <t>erreur en vertical + deux verticaux dispo + minimum un horizontal utilisé</t>
   </si>
 </sst>
 </file>
@@ -589,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K6:AX94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" workbookViewId="0">
-      <selection activeCell="BB42" sqref="BB42"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="BK25" sqref="BK25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,6 +860,9 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="4"/>
+      <c r="AS12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="16:50" x14ac:dyDescent="0.3">
       <c r="P13" s="1"/>
@@ -850,6 +892,9 @@
       <c r="AN13" s="1"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="4"/>
+      <c r="AT13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="16:50" x14ac:dyDescent="0.3">
       <c r="P14" s="1"/>
@@ -879,6 +924,9 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="4"/>
+      <c r="AT14" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="16:50" x14ac:dyDescent="0.3">
       <c r="P15" s="1"/>
@@ -908,6 +956,9 @@
       <c r="AN15" s="1"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="4"/>
+      <c r="AU15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="16:50" x14ac:dyDescent="0.3">
       <c r="P16" s="1"/>
@@ -937,54 +988,93 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="4"/>
-    </row>
-    <row r="18" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="12:47" x14ac:dyDescent="0.3">
+      <c r="AU17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="12:47" x14ac:dyDescent="0.3">
       <c r="O18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="12:47" x14ac:dyDescent="0.3">
       <c r="O19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AT19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="12:47" x14ac:dyDescent="0.3">
       <c r="O20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="12:47" x14ac:dyDescent="0.3">
+      <c r="AU21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="12:47" x14ac:dyDescent="0.3">
+      <c r="AU22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S24" t="s">
         <v>6</v>
       </c>
       <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AT25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="12:37" x14ac:dyDescent="0.3">
+      <c r="AU26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="12:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="12:47" x14ac:dyDescent="0.3">
       <c r="S28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="12:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="12:47" x14ac:dyDescent="0.3">
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
@@ -1009,7 +1099,7 @@
       <c r="AH30" s="12"/>
       <c r="AI30" s="12"/>
     </row>
-    <row r="31" spans="12:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="12:47" x14ac:dyDescent="0.3">
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
@@ -1043,7 +1133,7 @@
       <c r="AH31" s="12"/>
       <c r="AI31" s="12"/>
     </row>
-    <row r="32" spans="12:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="12:47" x14ac:dyDescent="0.3">
       <c r="L32" s="12"/>
       <c r="M32" s="13"/>
       <c r="N32" s="14" t="s">

</xml_diff>

<commit_message>
Improved : _minimizeObjective, Added : test2 (knight pathfinding)
</commit_message>
<xml_diff>
--- a/reflexion IA.xlsx
+++ b/reflexion IA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11148" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="12360" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="94">
   <si>
     <t>algorithme avec 1 détour</t>
   </si>
@@ -287,6 +287,15 @@
   </si>
   <si>
     <t>28 déplacements</t>
+  </si>
+  <si>
+    <t>distance =</t>
+  </si>
+  <si>
+    <t>détours =</t>
+  </si>
+  <si>
+    <t>prix =</t>
   </si>
 </sst>
 </file>
@@ -747,11 +756,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA90" sqref="AA90"/>
+    <sheetView tabSelected="1" topLeftCell="Q13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BK26" sqref="BK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="63" max="63" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="F1" t="s">
@@ -1447,22 +1459,26 @@
       <c r="AS24" s="1"/>
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
-      <c r="AV24" s="1"/>
-      <c r="AW24" s="1"/>
-      <c r="AX24" s="1"/>
-      <c r="AY24" s="1"/>
-      <c r="AZ24" s="1"/>
-      <c r="BA24" s="1"/>
-      <c r="BB24" s="1"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
       <c r="BE24" s="1"/>
       <c r="BF24" s="1"/>
-      <c r="BG24" s="1"/>
+      <c r="BG24" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="BH24" s="1"/>
       <c r="BI24" s="1"/>
       <c r="BJ24" s="1"/>
-      <c r="BK24" s="1"/>
+      <c r="BK24" s="1">
+        <v>2</v>
+      </c>
       <c r="BL24" s="1"/>
       <c r="BM24" s="1"/>
       <c r="BN24" s="1"/>
@@ -1539,22 +1555,38 @@
       <c r="AS25" s="1"/>
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
-      <c r="AV25" s="1"/>
-      <c r="AW25" s="1"/>
-      <c r="AX25" s="1"/>
-      <c r="AY25" s="1"/>
-      <c r="AZ25" s="1"/>
-      <c r="BA25" s="1"/>
-      <c r="BB25" s="1"/>
-      <c r="BC25" s="1"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="25">
+        <v>5</v>
+      </c>
+      <c r="AX25" s="25">
+        <v>4</v>
+      </c>
+      <c r="AY25" s="25">
+        <v>3</v>
+      </c>
+      <c r="AZ25" s="25">
+        <v>2</v>
+      </c>
+      <c r="BA25" s="25">
+        <v>1</v>
+      </c>
+      <c r="BB25" s="22">
+        <v>0</v>
+      </c>
+      <c r="BC25" s="2"/>
       <c r="BD25" s="1"/>
       <c r="BE25" s="1"/>
       <c r="BF25" s="1"/>
-      <c r="BG25" s="1"/>
+      <c r="BG25" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="BH25" s="1"/>
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
+      <c r="BK25" s="1">
+        <v>1</v>
+      </c>
       <c r="BL25" s="1"/>
       <c r="BM25" s="1"/>
       <c r="BN25" s="1"/>
@@ -1631,22 +1663,28 @@
       <c r="AS26" s="1"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
-      <c r="AV26" s="1"/>
-      <c r="AW26" s="1"/>
-      <c r="AX26" s="1"/>
-      <c r="AY26" s="1"/>
-      <c r="AZ26" s="1"/>
-      <c r="BA26" s="1"/>
-      <c r="BB26" s="1"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
       <c r="BF26" s="1"/>
-      <c r="BG26" s="1"/>
+      <c r="BG26" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="BH26" s="1"/>
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1"/>
-      <c r="BK26" s="1"/>
+      <c r="BK26" s="1">
+        <v>4</v>
+      </c>
       <c r="BL26" s="1"/>
       <c r="BM26" s="1"/>
       <c r="BN26" s="1"/>
@@ -1721,13 +1759,25 @@
       <c r="AS27" s="1"/>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
-      <c r="AV27" s="1"/>
-      <c r="AW27" s="1"/>
-      <c r="AX27" s="1"/>
-      <c r="AY27" s="1"/>
-      <c r="AZ27" s="1"/>
-      <c r="BA27" s="1"/>
-      <c r="BB27" s="1"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="4">
+        <v>5</v>
+      </c>
+      <c r="AX27" s="4">
+        <v>4</v>
+      </c>
+      <c r="AY27" s="4">
+        <v>3</v>
+      </c>
+      <c r="AZ27" s="4">
+        <v>2</v>
+      </c>
+      <c r="BA27" s="4">
+        <v>1</v>
+      </c>
+      <c r="BB27" s="23">
+        <v>2</v>
+      </c>
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
       <c r="BE27" s="1"/>
@@ -1807,13 +1857,13 @@
       <c r="AS28" s="1"/>
       <c r="AT28" s="1"/>
       <c r="AU28" s="1"/>
-      <c r="AV28" s="1"/>
-      <c r="AW28" s="1"/>
-      <c r="AX28" s="1"/>
-      <c r="AY28" s="1"/>
-      <c r="AZ28" s="1"/>
-      <c r="BA28" s="1"/>
-      <c r="BB28" s="1"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
       <c r="BC28" s="1"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1"/>

</xml_diff>

<commit_message>
Modified : PATHFINDING manage killings, Added : test3
</commit_message>
<xml_diff>
--- a/reflexion IA.xlsx
+++ b/reflexion IA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="14784" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="109">
   <si>
     <t>algorithme avec 1 détour</t>
   </si>
@@ -296,13 +296,58 @@
   </si>
   <si>
     <t>prix =</t>
+  </si>
+  <si>
+    <t>Réflexion Radar roi</t>
+  </si>
+  <si>
+    <t>5 AP</t>
+  </si>
+  <si>
+    <t>distance 1</t>
+  </si>
+  <si>
+    <t>si roof +1 distance</t>
+  </si>
+  <si>
+    <t>boucler</t>
+  </si>
+  <si>
+    <t>extremes + 1, test roof</t>
+  </si>
+  <si>
+    <t>dictionnaire des extremes avec 1 ou 2 direction(s)</t>
+  </si>
+  <si>
+    <t>si une direction, on cherche dans 3</t>
+  </si>
+  <si>
+    <t>si deux directions, on cherche dans 2</t>
+  </si>
+  <si>
+    <t>il y a des doublons de traitement, mais c'est ok car il faut tester</t>
+  </si>
+  <si>
+    <t>le passage G-R</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>test3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,8 +375,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +483,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -423,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -450,6 +553,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BK26" sqref="BK26"/>
+    <sheetView tabSelected="1" topLeftCell="AS33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BN42" sqref="BN42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,22 +881,66 @@
     <col min="63" max="63" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.3">
       <c r="F1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR1" s="26"/>
+    </row>
+    <row r="2" spans="1:75" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR2" s="26"/>
+      <c r="AV2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
       <c r="F3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR3" s="26"/>
+    </row>
+    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="AR4" s="26"/>
+    </row>
+    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+      <c r="AR5" s="26"/>
+      <c r="AV5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="1"/>
+      <c r="BV5" s="1"/>
+      <c r="BW5" s="1"/>
+    </row>
+    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -811,8 +971,57 @@
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR6" s="26"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH6" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BQ6" s="1"/>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+      <c r="BV6" s="1"/>
+      <c r="BW6" s="1"/>
+    </row>
+    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -843,8 +1052,57 @@
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
       <c r="AP7" s="1"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR7" s="26"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG7" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH7" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI7" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+      <c r="BT7" s="1"/>
+      <c r="BU7" s="1"/>
+      <c r="BV7" s="1"/>
+      <c r="BW7" s="1"/>
+    </row>
+    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -875,8 +1133,57 @@
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
       <c r="AP8" s="1"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR8" s="26"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BF8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BG8" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH8" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI8" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
+      <c r="BV8" s="1"/>
+      <c r="BW8" s="1"/>
+    </row>
+    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -904,8 +1211,37 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR9" s="26"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="30"/>
+      <c r="BG9" s="29"/>
+      <c r="BH9" s="27"/>
+      <c r="BI9" s="29"/>
+      <c r="BJ9" s="30"/>
+      <c r="BK9" s="30"/>
+      <c r="BL9" s="1"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+      <c r="BQ9" s="1"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+      <c r="BT9" s="1"/>
+      <c r="BU9" s="1"/>
+      <c r="BV9" s="1"/>
+      <c r="BW9" s="1"/>
+    </row>
+    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
       <c r="P10" s="1"/>
       <c r="Q10" s="22"/>
       <c r="R10" s="5"/>
@@ -933,8 +1269,37 @@
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
       <c r="AP10" s="1"/>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR10" s="26"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="30"/>
+      <c r="BF10" s="29"/>
+      <c r="BG10" s="27"/>
+      <c r="BH10" s="28"/>
+      <c r="BI10" s="27"/>
+      <c r="BJ10" s="29"/>
+      <c r="BK10" s="29"/>
+      <c r="BL10" s="30"/>
+      <c r="BM10" s="30"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+      <c r="BQ10" s="1"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+      <c r="BT10" s="1"/>
+      <c r="BU10" s="1"/>
+      <c r="BV10" s="1"/>
+      <c r="BW10" s="1"/>
+    </row>
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="20"/>
@@ -962,8 +1327,43 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
       <c r="AP11" s="1"/>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR11" s="26"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="30"/>
+      <c r="BE11" s="29"/>
+      <c r="BF11" s="27"/>
+      <c r="BG11" s="28"/>
+      <c r="BH11" s="23"/>
+      <c r="BI11" s="28"/>
+      <c r="BJ11" s="27"/>
+      <c r="BK11" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL11" s="29"/>
+      <c r="BM11" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN11" s="30"/>
+      <c r="BO11" s="1"/>
+      <c r="BP11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BQ11" s="1"/>
+      <c r="BR11" s="1"/>
+      <c r="BS11" s="1"/>
+      <c r="BT11" s="1"/>
+      <c r="BU11" s="1"/>
+      <c r="BV11" s="1"/>
+      <c r="BW11" s="1"/>
+    </row>
+    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -994,8 +1394,39 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR12" s="26"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="30"/>
+      <c r="BF12" s="29"/>
+      <c r="BG12" s="27"/>
+      <c r="BH12" s="28"/>
+      <c r="BI12" s="27"/>
+      <c r="BJ12" s="29"/>
+      <c r="BK12" s="29"/>
+      <c r="BL12" s="30"/>
+      <c r="BM12" s="30"/>
+      <c r="BN12" s="1"/>
+      <c r="BO12" s="1"/>
+      <c r="BP12" s="1"/>
+      <c r="BQ12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BR12" s="1"/>
+      <c r="BS12" s="1"/>
+      <c r="BT12" s="1"/>
+      <c r="BU12" s="1"/>
+      <c r="BV12" s="1"/>
+      <c r="BW12" s="1"/>
+    </row>
+    <row r="13" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1026,8 +1457,41 @@
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
       <c r="AP13" s="1"/>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR13" s="26"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="30"/>
+      <c r="BF13" s="29"/>
+      <c r="BG13" s="27"/>
+      <c r="BH13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI13" s="27"/>
+      <c r="BJ13" s="29"/>
+      <c r="BK13" s="30"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="1"/>
+      <c r="BP13" s="1"/>
+      <c r="BQ13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR13" s="1"/>
+      <c r="BS13" s="1"/>
+      <c r="BT13" s="1"/>
+      <c r="BU13" s="1"/>
+      <c r="BV13" s="1"/>
+      <c r="BW13" s="1"/>
+    </row>
+    <row r="14" spans="1:75" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>72</v>
       </c>
@@ -1058,8 +1522,39 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR14" s="26"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="30"/>
+      <c r="BG14" s="29"/>
+      <c r="BH14" s="27"/>
+      <c r="BI14" s="29"/>
+      <c r="BJ14" s="30"/>
+      <c r="BK14" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+      <c r="BO14" s="1"/>
+      <c r="BP14" s="1"/>
+      <c r="BQ14" s="1"/>
+      <c r="BR14" s="1"/>
+      <c r="BS14" s="1"/>
+      <c r="BT14" s="1"/>
+      <c r="BU14" s="1"/>
+      <c r="BV14" s="1"/>
+      <c r="BW14" s="1"/>
+    </row>
+    <row r="15" spans="1:75" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>66</v>
       </c>
@@ -1090,8 +1585,43 @@
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="AR15" s="26"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="30"/>
+      <c r="BG15" s="29"/>
+      <c r="BH15" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI15" s="29"/>
+      <c r="BJ15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK15" s="30"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BQ15" s="1"/>
+      <c r="BR15" s="1"/>
+      <c r="BS15" s="1"/>
+      <c r="BT15" s="1"/>
+      <c r="BU15" s="1"/>
+      <c r="BV15" s="1"/>
+      <c r="BW15" s="1"/>
+    </row>
+    <row r="16" spans="1:75" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>67</v>
       </c>
@@ -1122,26 +1652,151 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
+      <c r="AR16" s="26"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="30"/>
+      <c r="BH16" s="29"/>
+      <c r="BI16" s="30"/>
+      <c r="BJ16" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK16" s="1"/>
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+      <c r="BP16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BQ16" s="1"/>
+      <c r="BR16" s="1"/>
+      <c r="BS16" s="1"/>
+      <c r="BT16" s="1"/>
+      <c r="BU16" s="1"/>
+      <c r="BV16" s="1"/>
+      <c r="BW16" s="1"/>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>68</v>
       </c>
+      <c r="AR17" s="26"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="30"/>
+      <c r="BH17" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI17" s="30"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+      <c r="BP17" s="1"/>
+      <c r="BQ17" s="1"/>
+      <c r="BR17" s="1"/>
+      <c r="BS17" s="1"/>
+      <c r="BT17" s="1"/>
+      <c r="BU17" s="1"/>
+      <c r="BV17" s="1"/>
+      <c r="BW17" s="1"/>
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>69</v>
       </c>
+      <c r="AR18" s="26"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1"/>
+      <c r="BD18" s="1"/>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="1"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="30"/>
+      <c r="BI18" s="1"/>
+      <c r="BJ18" s="1"/>
+      <c r="BK18" s="1"/>
+      <c r="BL18" s="1"/>
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+      <c r="BO18" s="1"/>
+      <c r="BP18" s="1"/>
+      <c r="BQ18" s="1"/>
+      <c r="BR18" s="1"/>
+      <c r="BS18" s="1"/>
+      <c r="BT18" s="1"/>
+      <c r="BU18" s="1"/>
+      <c r="BV18" s="1"/>
+      <c r="BW18" s="1"/>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>70</v>
       </c>
+      <c r="AR19" s="26"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="BI19" s="1"/>
+      <c r="BJ19" s="1"/>
+      <c r="BK19" s="1"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+      <c r="BO19" s="1"/>
+      <c r="BP19" s="1"/>
+      <c r="BQ19" s="1"/>
+      <c r="BR19" s="1"/>
+      <c r="BS19" s="1"/>
+      <c r="BT19" s="1"/>
+      <c r="BU19" s="1"/>
+      <c r="BV19" s="1"/>
+      <c r="BW19" s="1"/>
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>71</v>
       </c>
+      <c r="AR20" s="26"/>
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
@@ -1585,7 +2240,7 @@
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1"/>
       <c r="BK25" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="BL25" s="1"/>
       <c r="BM25" s="1"/>
@@ -1683,7 +2338,7 @@
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1"/>
       <c r="BK26" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="BL26" s="1"/>
       <c r="BM26" s="1"/>
@@ -2115,7 +2770,9 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
-      <c r="AP31" s="1"/>
+      <c r="AP31" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
       <c r="AS31" s="1"/>
@@ -2129,7 +2786,9 @@
       <c r="BA31" s="1"/>
       <c r="BB31" s="1"/>
       <c r="BC31" s="1"/>
-      <c r="BD31" s="1"/>
+      <c r="BD31" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="BE31" s="1"/>
       <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
@@ -2203,32 +2862,32 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
       <c r="AO32" s="1"/>
-      <c r="AP32" s="1"/>
-      <c r="AQ32" s="1"/>
-      <c r="AR32" s="1"/>
-      <c r="AS32" s="1"/>
-      <c r="AT32" s="1"/>
-      <c r="AU32" s="1"/>
-      <c r="AV32" s="1"/>
-      <c r="AW32" s="1"/>
-      <c r="AX32" s="1"/>
-      <c r="AY32" s="1"/>
-      <c r="AZ32" s="1"/>
-      <c r="BA32" s="1"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+      <c r="AX32" s="2"/>
+      <c r="AY32" s="2"/>
+      <c r="AZ32" s="2"/>
+      <c r="BA32" s="2"/>
       <c r="BB32" s="1"/>
       <c r="BC32" s="1"/>
-      <c r="BD32" s="1"/>
-      <c r="BE32" s="1"/>
-      <c r="BF32" s="1"/>
-      <c r="BG32" s="1"/>
-      <c r="BH32" s="1"/>
-      <c r="BI32" s="1"/>
-      <c r="BJ32" s="1"/>
-      <c r="BK32" s="1"/>
-      <c r="BL32" s="1"/>
-      <c r="BM32" s="1"/>
-      <c r="BN32" s="1"/>
-      <c r="BO32" s="1"/>
+      <c r="BD32" s="2"/>
+      <c r="BE32" s="2"/>
+      <c r="BF32" s="2"/>
+      <c r="BG32" s="2"/>
+      <c r="BH32" s="2"/>
+      <c r="BI32" s="2"/>
+      <c r="BJ32" s="2"/>
+      <c r="BK32" s="2"/>
+      <c r="BL32" s="2"/>
+      <c r="BM32" s="2"/>
+      <c r="BN32" s="2"/>
+      <c r="BO32" s="2"/>
       <c r="BP32" s="1"/>
       <c r="BQ32" s="1"/>
       <c r="BR32" s="1"/>
@@ -2291,7 +2950,7 @@
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
-      <c r="AP33" s="1"/>
+      <c r="AP33" s="2"/>
       <c r="AQ33" s="1"/>
       <c r="AR33" s="1"/>
       <c r="AS33" s="1"/>
@@ -2302,21 +2961,21 @@
       <c r="AX33" s="1"/>
       <c r="AY33" s="1"/>
       <c r="AZ33" s="1"/>
-      <c r="BA33" s="1"/>
+      <c r="BA33" s="2"/>
       <c r="BB33" s="1"/>
       <c r="BC33" s="1"/>
-      <c r="BD33" s="1"/>
-      <c r="BE33" s="1"/>
-      <c r="BF33" s="1"/>
-      <c r="BG33" s="1"/>
-      <c r="BH33" s="1"/>
-      <c r="BI33" s="1"/>
-      <c r="BJ33" s="1"/>
-      <c r="BK33" s="1"/>
-      <c r="BL33" s="1"/>
-      <c r="BM33" s="1"/>
-      <c r="BN33" s="1"/>
-      <c r="BO33" s="1"/>
+      <c r="BD33" s="2"/>
+      <c r="BE33" s="32"/>
+      <c r="BF33" s="32"/>
+      <c r="BG33" s="32"/>
+      <c r="BH33" s="32"/>
+      <c r="BI33" s="32"/>
+      <c r="BJ33" s="32"/>
+      <c r="BK33" s="32"/>
+      <c r="BL33" s="32"/>
+      <c r="BM33" s="32"/>
+      <c r="BN33" s="32"/>
+      <c r="BO33" s="2"/>
       <c r="BP33" s="1"/>
       <c r="BQ33" s="1"/>
       <c r="BR33" s="1"/>
@@ -2379,7 +3038,7 @@
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
-      <c r="AP34" s="1"/>
+      <c r="AP34" s="2"/>
       <c r="AQ34" s="1"/>
       <c r="AR34" s="1"/>
       <c r="AS34" s="1"/>
@@ -2390,21 +3049,21 @@
       <c r="AX34" s="1"/>
       <c r="AY34" s="1"/>
       <c r="AZ34" s="1"/>
-      <c r="BA34" s="1"/>
+      <c r="BA34" s="2"/>
       <c r="BB34" s="1"/>
       <c r="BC34" s="1"/>
-      <c r="BD34" s="1"/>
-      <c r="BE34" s="1"/>
-      <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
-      <c r="BH34" s="1"/>
-      <c r="BI34" s="1"/>
-      <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
-      <c r="BL34" s="1"/>
-      <c r="BM34" s="1"/>
-      <c r="BN34" s="1"/>
-      <c r="BO34" s="1"/>
+      <c r="BD34" s="2"/>
+      <c r="BE34" s="32"/>
+      <c r="BF34" s="32"/>
+      <c r="BG34" s="32"/>
+      <c r="BH34" s="32"/>
+      <c r="BI34" s="32"/>
+      <c r="BJ34" s="32"/>
+      <c r="BK34" s="32"/>
+      <c r="BL34" s="32"/>
+      <c r="BM34" s="32"/>
+      <c r="BN34" s="32"/>
+      <c r="BO34" s="2"/>
       <c r="BP34" s="1"/>
       <c r="BQ34" s="1"/>
       <c r="BR34" s="1"/>
@@ -2465,7 +3124,7 @@
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
-      <c r="AP35" s="1"/>
+      <c r="AP35" s="2"/>
       <c r="AQ35" s="1"/>
       <c r="AR35" s="1"/>
       <c r="AS35" s="1"/>
@@ -2476,21 +3135,21 @@
       <c r="AX35" s="1"/>
       <c r="AY35" s="1"/>
       <c r="AZ35" s="1"/>
-      <c r="BA35" s="1"/>
+      <c r="BA35" s="2"/>
       <c r="BB35" s="1"/>
       <c r="BC35" s="1"/>
-      <c r="BD35" s="1"/>
-      <c r="BE35" s="1"/>
-      <c r="BF35" s="1"/>
-      <c r="BG35" s="1"/>
-      <c r="BH35" s="1"/>
-      <c r="BI35" s="1"/>
-      <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
-      <c r="BL35" s="1"/>
-      <c r="BM35" s="1"/>
-      <c r="BN35" s="1"/>
-      <c r="BO35" s="1"/>
+      <c r="BD35" s="2"/>
+      <c r="BE35" s="32"/>
+      <c r="BF35" s="32"/>
+      <c r="BG35" s="32"/>
+      <c r="BH35" s="32"/>
+      <c r="BI35" s="32"/>
+      <c r="BJ35" s="32"/>
+      <c r="BK35" s="32"/>
+      <c r="BL35" s="32"/>
+      <c r="BM35" s="32"/>
+      <c r="BN35" s="32"/>
+      <c r="BO35" s="2"/>
       <c r="BP35" s="1"/>
       <c r="BQ35" s="1"/>
       <c r="BR35" s="1"/>
@@ -2551,7 +3210,7 @@
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
-      <c r="AP36" s="1"/>
+      <c r="AP36" s="2"/>
       <c r="AQ36" s="1"/>
       <c r="AR36" s="1"/>
       <c r="AS36" s="1"/>
@@ -2562,21 +3221,21 @@
       <c r="AX36" s="1"/>
       <c r="AY36" s="1"/>
       <c r="AZ36" s="1"/>
-      <c r="BA36" s="1"/>
+      <c r="BA36" s="2"/>
       <c r="BB36" s="1"/>
       <c r="BC36" s="1"/>
-      <c r="BD36" s="1"/>
-      <c r="BE36" s="1"/>
-      <c r="BF36" s="1"/>
-      <c r="BG36" s="1"/>
-      <c r="BH36" s="1"/>
-      <c r="BI36" s="1"/>
-      <c r="BJ36" s="1"/>
-      <c r="BK36" s="1"/>
-      <c r="BL36" s="1"/>
-      <c r="BM36" s="1"/>
-      <c r="BN36" s="1"/>
-      <c r="BO36" s="1"/>
+      <c r="BD36" s="2"/>
+      <c r="BE36" s="32"/>
+      <c r="BF36" s="32"/>
+      <c r="BG36" s="32"/>
+      <c r="BH36" s="32"/>
+      <c r="BI36" s="32"/>
+      <c r="BJ36" s="32"/>
+      <c r="BK36" s="32"/>
+      <c r="BL36" s="32"/>
+      <c r="BM36" s="32"/>
+      <c r="BN36" s="32"/>
+      <c r="BO36" s="2"/>
       <c r="BP36" s="1"/>
       <c r="BQ36" s="1"/>
       <c r="BR36" s="1"/>
@@ -2639,32 +3298,48 @@
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
-      <c r="AP37" s="1"/>
+      <c r="AP37" s="2"/>
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>
       <c r="AS37" s="1"/>
-      <c r="AT37" s="1"/>
-      <c r="AU37" s="1"/>
-      <c r="AV37" s="1"/>
-      <c r="AW37" s="1"/>
+      <c r="AT37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU37" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV37" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW37" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="AX37" s="1"/>
       <c r="AY37" s="1"/>
       <c r="AZ37" s="1"/>
-      <c r="BA37" s="1"/>
+      <c r="BA37" s="2"/>
       <c r="BB37" s="1"/>
       <c r="BC37" s="1"/>
-      <c r="BD37" s="1"/>
-      <c r="BE37" s="1"/>
-      <c r="BF37" s="1"/>
-      <c r="BG37" s="1"/>
-      <c r="BH37" s="1"/>
-      <c r="BI37" s="1"/>
-      <c r="BJ37" s="1"/>
-      <c r="BK37" s="1"/>
-      <c r="BL37" s="1"/>
-      <c r="BM37" s="1"/>
-      <c r="BN37" s="1"/>
-      <c r="BO37" s="1"/>
+      <c r="BD37" s="2"/>
+      <c r="BE37" s="32"/>
+      <c r="BF37" s="32"/>
+      <c r="BG37" s="32"/>
+      <c r="BH37" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI37" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="BJ37" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK37" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BL37" s="32"/>
+      <c r="BM37" s="32"/>
+      <c r="BN37" s="32"/>
+      <c r="BO37" s="2"/>
       <c r="BP37" s="1"/>
       <c r="BQ37" s="1"/>
       <c r="BR37" s="1"/>
@@ -2727,32 +3402,42 @@
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
-      <c r="AP38" s="1"/>
+      <c r="AP38" s="2"/>
       <c r="AQ38" s="1"/>
       <c r="AR38" s="1"/>
       <c r="AS38" s="1"/>
       <c r="AT38" s="1"/>
-      <c r="AU38" s="1"/>
-      <c r="AV38" s="1"/>
+      <c r="AU38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV38" s="5"/>
       <c r="AW38" s="1"/>
       <c r="AX38" s="1"/>
-      <c r="AY38" s="1"/>
+      <c r="AY38" s="35" t="s">
+        <v>107</v>
+      </c>
       <c r="AZ38" s="1"/>
-      <c r="BA38" s="1"/>
+      <c r="BA38" s="2"/>
       <c r="BB38" s="1"/>
       <c r="BC38" s="1"/>
-      <c r="BD38" s="1"/>
-      <c r="BE38" s="1"/>
-      <c r="BF38" s="1"/>
-      <c r="BG38" s="1"/>
-      <c r="BH38" s="1"/>
-      <c r="BI38" s="1"/>
-      <c r="BJ38" s="1"/>
-      <c r="BK38" s="1"/>
-      <c r="BL38" s="1"/>
-      <c r="BM38" s="1"/>
-      <c r="BN38" s="1"/>
-      <c r="BO38" s="1"/>
+      <c r="BD38" s="2"/>
+      <c r="BE38" s="32"/>
+      <c r="BF38" s="32"/>
+      <c r="BG38" s="32"/>
+      <c r="BH38" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI38" s="31"/>
+      <c r="BJ38" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK38" s="31"/>
+      <c r="BL38" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="BM38" s="32"/>
+      <c r="BN38" s="32"/>
+      <c r="BO38" s="2"/>
       <c r="BP38" s="1"/>
       <c r="BQ38" s="1"/>
       <c r="BR38" s="1"/>
@@ -2813,32 +3498,44 @@
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
-      <c r="AP39" s="1"/>
+      <c r="AP39" s="2"/>
       <c r="AQ39" s="1"/>
       <c r="AR39" s="1"/>
       <c r="AS39" s="1"/>
       <c r="AT39" s="1"/>
-      <c r="AU39" s="1"/>
-      <c r="AV39" s="1"/>
+      <c r="AU39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV39" s="5"/>
       <c r="AW39" s="1"/>
       <c r="AX39" s="1"/>
-      <c r="AY39" s="1"/>
-      <c r="AZ39" s="1"/>
-      <c r="BA39" s="1"/>
+      <c r="AY39" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA39" s="2"/>
       <c r="BB39" s="1"/>
       <c r="BC39" s="1"/>
-      <c r="BD39" s="1"/>
-      <c r="BE39" s="1"/>
-      <c r="BF39" s="1"/>
-      <c r="BG39" s="1"/>
-      <c r="BH39" s="1"/>
-      <c r="BI39" s="1"/>
-      <c r="BJ39" s="1"/>
-      <c r="BK39" s="1"/>
-      <c r="BL39" s="1"/>
-      <c r="BM39" s="1"/>
-      <c r="BN39" s="1"/>
-      <c r="BO39" s="1"/>
+      <c r="BD39" s="2"/>
+      <c r="BE39" s="32"/>
+      <c r="BF39" s="32"/>
+      <c r="BG39" s="32"/>
+      <c r="BH39" s="32"/>
+      <c r="BI39" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ39" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK39" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL39" s="31"/>
+      <c r="BM39" s="32"/>
+      <c r="BN39" s="32"/>
+      <c r="BO39" s="2"/>
       <c r="BP39" s="1"/>
       <c r="BQ39" s="1"/>
       <c r="BR39" s="1"/>
@@ -2899,32 +3596,48 @@
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
       <c r="AO40" s="1"/>
-      <c r="AP40" s="1"/>
+      <c r="AP40" s="2"/>
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
       <c r="AS40" s="1"/>
       <c r="AT40" s="1"/>
-      <c r="AU40" s="1"/>
-      <c r="AV40" s="1"/>
-      <c r="AW40" s="1"/>
-      <c r="AX40" s="1"/>
-      <c r="AY40" s="1"/>
-      <c r="AZ40" s="1"/>
-      <c r="BA40" s="1"/>
+      <c r="AU40" s="4"/>
+      <c r="AV40" s="5"/>
+      <c r="AW40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY40" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA40" s="2"/>
       <c r="BB40" s="1"/>
       <c r="BC40" s="1"/>
-      <c r="BD40" s="1"/>
-      <c r="BE40" s="1"/>
-      <c r="BF40" s="1"/>
-      <c r="BG40" s="1"/>
-      <c r="BH40" s="1"/>
-      <c r="BI40" s="1"/>
-      <c r="BJ40" s="1"/>
-      <c r="BK40" s="1"/>
-      <c r="BL40" s="1"/>
-      <c r="BM40" s="1"/>
-      <c r="BN40" s="1"/>
-      <c r="BO40" s="1"/>
+      <c r="BD40" s="2"/>
+      <c r="BE40" s="32"/>
+      <c r="BF40" s="32"/>
+      <c r="BG40" s="32"/>
+      <c r="BH40" s="32"/>
+      <c r="BI40" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ40" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK40" s="11"/>
+      <c r="BL40" s="31"/>
+      <c r="BM40" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN40" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BO40" s="2"/>
       <c r="BP40" s="1"/>
       <c r="BQ40" s="1"/>
       <c r="BR40" s="1"/>
@@ -2985,32 +3698,48 @@
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
       <c r="AO41" s="1"/>
-      <c r="AP41" s="1"/>
+      <c r="AP41" s="2"/>
       <c r="AQ41" s="1"/>
       <c r="AR41" s="1"/>
       <c r="AS41" s="1"/>
       <c r="AT41" s="1"/>
-      <c r="AU41" s="1"/>
-      <c r="AV41" s="1"/>
-      <c r="AW41" s="1"/>
-      <c r="AX41" s="1"/>
-      <c r="AY41" s="1"/>
-      <c r="AZ41" s="1"/>
-      <c r="BA41" s="1"/>
+      <c r="AU41" s="5"/>
+      <c r="AV41" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW41" s="5"/>
+      <c r="AX41" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY41" s="34"/>
+      <c r="AZ41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="BA41" s="2"/>
       <c r="BB41" s="1"/>
       <c r="BC41" s="1"/>
-      <c r="BD41" s="1"/>
-      <c r="BE41" s="1"/>
-      <c r="BF41" s="1"/>
-      <c r="BG41" s="1"/>
-      <c r="BH41" s="1"/>
-      <c r="BI41" s="1"/>
-      <c r="BJ41" s="1"/>
-      <c r="BK41" s="1"/>
-      <c r="BL41" s="1"/>
-      <c r="BM41" s="1"/>
-      <c r="BN41" s="1"/>
-      <c r="BO41" s="1"/>
+      <c r="BD41" s="2"/>
+      <c r="BE41" s="32"/>
+      <c r="BF41" s="32"/>
+      <c r="BG41" s="32"/>
+      <c r="BH41" s="32"/>
+      <c r="BI41" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ41" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK41" s="31"/>
+      <c r="BL41" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM41" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN41" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BO41" s="2"/>
       <c r="BP41" s="1"/>
       <c r="BQ41" s="1"/>
       <c r="BR41" s="1"/>
@@ -3071,32 +3800,48 @@
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
       <c r="AO42" s="1"/>
-      <c r="AP42" s="1"/>
+      <c r="AP42" s="2"/>
       <c r="AQ42" s="1"/>
       <c r="AR42" s="1"/>
       <c r="AS42" s="1"/>
       <c r="AT42" s="1"/>
-      <c r="AU42" s="1"/>
-      <c r="AV42" s="1"/>
-      <c r="AW42" s="1"/>
-      <c r="AX42" s="1"/>
-      <c r="AY42" s="1"/>
+      <c r="AU42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX42" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AY42" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="AZ42" s="1"/>
-      <c r="BA42" s="1"/>
+      <c r="BA42" s="2"/>
       <c r="BB42" s="1"/>
       <c r="BC42" s="1"/>
-      <c r="BD42" s="1"/>
-      <c r="BE42" s="1"/>
-      <c r="BF42" s="1"/>
-      <c r="BG42" s="1"/>
-      <c r="BH42" s="1"/>
-      <c r="BI42" s="1"/>
-      <c r="BJ42" s="1"/>
-      <c r="BK42" s="1"/>
-      <c r="BL42" s="1"/>
-      <c r="BM42" s="1"/>
-      <c r="BN42" s="1"/>
-      <c r="BO42" s="1"/>
+      <c r="BD42" s="2"/>
+      <c r="BE42" s="32"/>
+      <c r="BF42" s="32"/>
+      <c r="BG42" s="32"/>
+      <c r="BH42" s="32"/>
+      <c r="BI42" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BJ42" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK42" s="31"/>
+      <c r="BL42" s="31"/>
+      <c r="BM42" s="31"/>
+      <c r="BN42" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO42" s="2"/>
       <c r="BP42" s="1"/>
       <c r="BQ42" s="1"/>
       <c r="BR42" s="1"/>
@@ -3157,32 +3902,32 @@
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
       <c r="AO43" s="1"/>
-      <c r="AP43" s="1"/>
-      <c r="AQ43" s="1"/>
-      <c r="AR43" s="1"/>
-      <c r="AS43" s="1"/>
-      <c r="AT43" s="1"/>
-      <c r="AU43" s="1"/>
-      <c r="AV43" s="1"/>
-      <c r="AW43" s="1"/>
-      <c r="AX43" s="1"/>
-      <c r="AY43" s="1"/>
-      <c r="AZ43" s="1"/>
-      <c r="BA43" s="1"/>
+      <c r="AP43" s="2"/>
+      <c r="AQ43" s="2"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="2"/>
+      <c r="AT43" s="2"/>
+      <c r="AU43" s="2"/>
+      <c r="AV43" s="2"/>
+      <c r="AW43" s="2"/>
+      <c r="AX43" s="2"/>
+      <c r="AY43" s="2"/>
+      <c r="AZ43" s="2"/>
+      <c r="BA43" s="2"/>
       <c r="BB43" s="1"/>
       <c r="BC43" s="1"/>
-      <c r="BD43" s="1"/>
-      <c r="BE43" s="1"/>
-      <c r="BF43" s="1"/>
-      <c r="BG43" s="1"/>
-      <c r="BH43" s="1"/>
-      <c r="BI43" s="1"/>
-      <c r="BJ43" s="1"/>
-      <c r="BK43" s="1"/>
-      <c r="BL43" s="1"/>
-      <c r="BM43" s="1"/>
-      <c r="BN43" s="1"/>
-      <c r="BO43" s="1"/>
+      <c r="BD43" s="2"/>
+      <c r="BE43" s="2"/>
+      <c r="BF43" s="2"/>
+      <c r="BG43" s="2"/>
+      <c r="BH43" s="2"/>
+      <c r="BI43" s="2"/>
+      <c r="BJ43" s="2"/>
+      <c r="BK43" s="2"/>
+      <c r="BL43" s="2"/>
+      <c r="BM43" s="2"/>
+      <c r="BN43" s="2"/>
+      <c r="BO43" s="2"/>
       <c r="BP43" s="1"/>
       <c r="BQ43" s="1"/>
       <c r="BR43" s="1"/>

</xml_diff>

<commit_message>
Added _radarKingDefensive, _getcoords, test4 : Evaluates Threats to the king
</commit_message>
<xml_diff>
--- a/reflexion IA.xlsx
+++ b/reflexion IA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15996" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="18420" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="110">
   <si>
     <t>algorithme avec 1 détour</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
   </si>
 </sst>
 </file>
@@ -872,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="CB42" sqref="CB42"/>
+    <sheetView tabSelected="1" topLeftCell="AT7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BT39" sqref="BT39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2802,7 +2805,9 @@
       <c r="BO31" s="1"/>
       <c r="BP31" s="1"/>
       <c r="BQ31" s="1"/>
-      <c r="BR31" s="1"/>
+      <c r="BR31" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="BS31" s="1"/>
       <c r="BT31" s="1"/>
       <c r="BU31" s="1"/>
@@ -2890,18 +2895,18 @@
       <c r="BO32" s="2"/>
       <c r="BP32" s="1"/>
       <c r="BQ32" s="1"/>
-      <c r="BR32" s="1"/>
-      <c r="BS32" s="1"/>
-      <c r="BT32" s="1"/>
-      <c r="BU32" s="1"/>
-      <c r="BV32" s="1"/>
-      <c r="BW32" s="1"/>
-      <c r="BX32" s="1"/>
-      <c r="BY32" s="1"/>
-      <c r="BZ32" s="1"/>
-      <c r="CA32" s="1"/>
-      <c r="CB32" s="1"/>
-      <c r="CC32" s="1"/>
+      <c r="BR32" s="2"/>
+      <c r="BS32" s="2"/>
+      <c r="BT32" s="2"/>
+      <c r="BU32" s="2"/>
+      <c r="BV32" s="2"/>
+      <c r="BW32" s="2"/>
+      <c r="BX32" s="2"/>
+      <c r="BY32" s="2"/>
+      <c r="BZ32" s="2"/>
+      <c r="CA32" s="2"/>
+      <c r="CB32" s="2"/>
+      <c r="CC32" s="2"/>
       <c r="CD32" s="1"/>
       <c r="CE32" s="1"/>
       <c r="CF32" s="1"/>
@@ -2978,18 +2983,26 @@
       <c r="BO33" s="2"/>
       <c r="BP33" s="1"/>
       <c r="BQ33" s="1"/>
-      <c r="BR33" s="1"/>
-      <c r="BS33" s="1"/>
-      <c r="BT33" s="1"/>
-      <c r="BU33" s="1"/>
-      <c r="BV33" s="1"/>
-      <c r="BW33" s="1"/>
-      <c r="BX33" s="1"/>
-      <c r="BY33" s="1"/>
+      <c r="BR33" s="2"/>
+      <c r="BS33" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="BT33" s="28"/>
+      <c r="BU33" s="27"/>
+      <c r="BV33" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BW33" s="29"/>
+      <c r="BX33" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BY33" s="30" t="s">
+        <v>107</v>
+      </c>
       <c r="BZ33" s="1"/>
       <c r="CA33" s="1"/>
       <c r="CB33" s="1"/>
-      <c r="CC33" s="1"/>
+      <c r="CC33" s="2"/>
       <c r="CD33" s="1"/>
       <c r="CE33" s="1"/>
       <c r="CF33" s="1"/>
@@ -3066,18 +3079,20 @@
       <c r="BO34" s="2"/>
       <c r="BP34" s="1"/>
       <c r="BQ34" s="1"/>
-      <c r="BR34" s="1"/>
-      <c r="BS34" s="1"/>
-      <c r="BT34" s="1"/>
-      <c r="BU34" s="1"/>
-      <c r="BV34" s="1"/>
-      <c r="BW34" s="1"/>
-      <c r="BX34" s="1"/>
+      <c r="BR34" s="2"/>
+      <c r="BS34" s="28"/>
+      <c r="BT34" s="27"/>
+      <c r="BU34" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV34" s="29"/>
+      <c r="BW34" s="30"/>
+      <c r="BX34" s="30"/>
       <c r="BY34" s="1"/>
       <c r="BZ34" s="1"/>
       <c r="CA34" s="1"/>
       <c r="CB34" s="1"/>
-      <c r="CC34" s="1"/>
+      <c r="CC34" s="2"/>
       <c r="CD34" s="1"/>
       <c r="CE34" s="1"/>
       <c r="CF34" s="1"/>
@@ -3152,18 +3167,20 @@
       <c r="BO35" s="2"/>
       <c r="BP35" s="1"/>
       <c r="BQ35" s="1"/>
-      <c r="BR35" s="1"/>
-      <c r="BS35" s="1"/>
-      <c r="BT35" s="1"/>
-      <c r="BU35" s="1"/>
-      <c r="BV35" s="1"/>
+      <c r="BR35" s="2"/>
+      <c r="BS35" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT35" s="27"/>
+      <c r="BU35" s="29"/>
+      <c r="BV35" s="30"/>
       <c r="BW35" s="1"/>
       <c r="BX35" s="1"/>
       <c r="BY35" s="1"/>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
       <c r="CB35" s="1"/>
-      <c r="CC35" s="1"/>
+      <c r="CC35" s="2"/>
       <c r="CD35" s="1"/>
       <c r="CE35" s="1"/>
       <c r="CF35" s="1"/>
@@ -3238,18 +3255,22 @@
       <c r="BO36" s="2"/>
       <c r="BP36" s="1"/>
       <c r="BQ36" s="1"/>
-      <c r="BR36" s="1"/>
-      <c r="BS36" s="1"/>
-      <c r="BT36" s="1"/>
-      <c r="BU36" s="1"/>
-      <c r="BV36" s="1"/>
+      <c r="BR36" s="2"/>
+      <c r="BS36" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="BT36" s="29"/>
+      <c r="BU36" s="30"/>
+      <c r="BV36" s="30" t="s">
+        <v>2</v>
+      </c>
       <c r="BW36" s="1"/>
       <c r="BX36" s="1"/>
       <c r="BY36" s="1"/>
       <c r="BZ36" s="1"/>
       <c r="CA36" s="1"/>
       <c r="CB36" s="1"/>
-      <c r="CC36" s="1"/>
+      <c r="CC36" s="2"/>
       <c r="CD36" s="1"/>
       <c r="CE36" s="1"/>
       <c r="CF36" s="1"/>
@@ -3342,18 +3363,26 @@
       <c r="BO37" s="2"/>
       <c r="BP37" s="1"/>
       <c r="BQ37" s="1"/>
-      <c r="BR37" s="1"/>
-      <c r="BS37" s="1"/>
-      <c r="BT37" s="1"/>
-      <c r="BU37" s="1"/>
-      <c r="BV37" s="1"/>
+      <c r="BR37" s="2"/>
+      <c r="BS37" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT37" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="BU37" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BV37" s="30" t="s">
+        <v>106</v>
+      </c>
       <c r="BW37" s="1"/>
       <c r="BX37" s="1"/>
       <c r="BY37" s="1"/>
       <c r="BZ37" s="1"/>
       <c r="CA37" s="1"/>
       <c r="CB37" s="1"/>
-      <c r="CC37" s="1"/>
+      <c r="CC37" s="2"/>
       <c r="CD37" s="1"/>
       <c r="CE37" s="1"/>
       <c r="CF37" s="1"/>
@@ -3427,12 +3456,12 @@
       <c r="BH38" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="BI38" s="31"/>
-      <c r="BJ38" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="BK38" s="31"/>
-      <c r="BL38" s="31" t="s">
+      <c r="BI38" s="32"/>
+      <c r="BJ38" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="BK38" s="32"/>
+      <c r="BL38" s="36" t="s">
         <v>12</v>
       </c>
       <c r="BM38" s="32"/>
@@ -3440,10 +3469,12 @@
       <c r="BO38" s="2"/>
       <c r="BP38" s="1"/>
       <c r="BQ38" s="1"/>
-      <c r="BR38" s="1"/>
-      <c r="BS38" s="1"/>
-      <c r="BT38" s="1"/>
-      <c r="BU38" s="1"/>
+      <c r="BR38" s="2"/>
+      <c r="BS38" s="29"/>
+      <c r="BT38" s="30"/>
+      <c r="BU38" s="30" t="s">
+        <v>2</v>
+      </c>
       <c r="BV38" s="1"/>
       <c r="BW38" s="1"/>
       <c r="BX38" s="1"/>
@@ -3451,7 +3482,7 @@
       <c r="BZ38" s="1"/>
       <c r="CA38" s="1"/>
       <c r="CB38" s="1"/>
-      <c r="CC38" s="1"/>
+      <c r="CC38" s="2"/>
       <c r="CD38" s="1"/>
       <c r="CE38" s="1"/>
       <c r="CF38" s="1"/>
@@ -3538,9 +3569,11 @@
       <c r="BO39" s="2"/>
       <c r="BP39" s="1"/>
       <c r="BQ39" s="1"/>
-      <c r="BR39" s="1"/>
-      <c r="BS39" s="1"/>
-      <c r="BT39" s="1"/>
+      <c r="BR39" s="2"/>
+      <c r="BS39" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT39" s="30"/>
       <c r="BU39" s="1"/>
       <c r="BV39" s="1"/>
       <c r="BW39" s="1"/>
@@ -3549,7 +3582,7 @@
       <c r="BZ39" s="1"/>
       <c r="CA39" s="1"/>
       <c r="CB39" s="1"/>
-      <c r="CC39" s="1"/>
+      <c r="CC39" s="2"/>
       <c r="CD39" s="1"/>
       <c r="CE39" s="1"/>
       <c r="CF39" s="1"/>
@@ -3640,8 +3673,8 @@
       <c r="BO40" s="2"/>
       <c r="BP40" s="1"/>
       <c r="BQ40" s="1"/>
-      <c r="BR40" s="1"/>
-      <c r="BS40" s="1"/>
+      <c r="BR40" s="2"/>
+      <c r="BS40" s="30"/>
       <c r="BT40" s="1"/>
       <c r="BU40" s="1"/>
       <c r="BV40" s="1"/>
@@ -3651,7 +3684,7 @@
       <c r="BZ40" s="1"/>
       <c r="CA40" s="1"/>
       <c r="CB40" s="1"/>
-      <c r="CC40" s="1"/>
+      <c r="CC40" s="2"/>
       <c r="CD40" s="1"/>
       <c r="CE40" s="1"/>
       <c r="CF40" s="1"/>
@@ -3742,8 +3775,10 @@
       <c r="BO41" s="2"/>
       <c r="BP41" s="1"/>
       <c r="BQ41" s="1"/>
-      <c r="BR41" s="1"/>
-      <c r="BS41" s="1"/>
+      <c r="BR41" s="2"/>
+      <c r="BS41" s="30" t="s">
+        <v>2</v>
+      </c>
       <c r="BT41" s="1"/>
       <c r="BU41" s="1"/>
       <c r="BV41" s="1"/>
@@ -3753,7 +3788,7 @@
       <c r="BZ41" s="1"/>
       <c r="CA41" s="1"/>
       <c r="CB41" s="1"/>
-      <c r="CC41" s="1"/>
+      <c r="CC41" s="2"/>
       <c r="CD41" s="1"/>
       <c r="CE41" s="1"/>
       <c r="CF41" s="1"/>
@@ -3844,7 +3879,7 @@
       <c r="BO42" s="2"/>
       <c r="BP42" s="1"/>
       <c r="BQ42" s="1"/>
-      <c r="BR42" s="1"/>
+      <c r="BR42" s="2"/>
       <c r="BS42" s="1"/>
       <c r="BT42" s="1"/>
       <c r="BU42" s="1"/>
@@ -3855,7 +3890,7 @@
       <c r="BZ42" s="1"/>
       <c r="CA42" s="1"/>
       <c r="CB42" s="1"/>
-      <c r="CC42" s="1"/>
+      <c r="CC42" s="2"/>
       <c r="CD42" s="1"/>
       <c r="CE42" s="1"/>
       <c r="CF42" s="1"/>
@@ -3930,18 +3965,18 @@
       <c r="BO43" s="2"/>
       <c r="BP43" s="1"/>
       <c r="BQ43" s="1"/>
-      <c r="BR43" s="1"/>
-      <c r="BS43" s="1"/>
-      <c r="BT43" s="1"/>
-      <c r="BU43" s="1"/>
-      <c r="BV43" s="1"/>
-      <c r="BW43" s="1"/>
-      <c r="BX43" s="1"/>
-      <c r="BY43" s="1"/>
-      <c r="BZ43" s="1"/>
-      <c r="CA43" s="1"/>
-      <c r="CB43" s="1"/>
-      <c r="CC43" s="1"/>
+      <c r="BR43" s="2"/>
+      <c r="BS43" s="2"/>
+      <c r="BT43" s="2"/>
+      <c r="BU43" s="2"/>
+      <c r="BV43" s="2"/>
+      <c r="BW43" s="2"/>
+      <c r="BX43" s="2"/>
+      <c r="BY43" s="2"/>
+      <c r="BZ43" s="2"/>
+      <c r="CA43" s="2"/>
+      <c r="CB43" s="2"/>
+      <c r="CC43" s="2"/>
       <c r="CD43" s="1"/>
       <c r="CE43" s="1"/>
       <c r="CF43" s="1"/>

</xml_diff>

<commit_message>
Modified _radarDefensive, Added test5, test6
</commit_message>
<xml_diff>
--- a/reflexion IA.xlsx
+++ b/reflexion IA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="20844" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="22056" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="50">
   <si>
     <t>R</t>
   </si>
@@ -115,9 +115,6 @@
     <t>test1 :</t>
   </si>
   <si>
-    <t>Réflexion Radar roi</t>
-  </si>
-  <si>
     <t>5 AP</t>
   </si>
   <si>
@@ -137,6 +134,36 @@
   </si>
   <si>
     <t>IA actuelle :</t>
+  </si>
+  <si>
+    <t>radar chevalier</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>radar roi</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>radar villageois</t>
+  </si>
+  <si>
+    <t>erreur :</t>
+  </si>
+  <si>
+    <t>actuel :</t>
+  </si>
+  <si>
+    <t>Kn</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>(corrigée)</t>
   </si>
 </sst>
 </file>
@@ -193,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +311,60 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -329,6 +410,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BN25" sqref="BN25"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BK40" sqref="BK40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,32 +734,38 @@
     <col min="63" max="63" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:71" x14ac:dyDescent="0.3">
       <c r="AQ1" s="5"/>
       <c r="AR1" s="5"/>
       <c r="AS1" s="5"/>
     </row>
-    <row r="2" spans="2:45" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
+    <row r="2" spans="2:71" x14ac:dyDescent="0.3">
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
       <c r="AS2" s="5"/>
     </row>
-    <row r="3" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:71" x14ac:dyDescent="0.3">
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
       <c r="AS3" s="5"/>
     </row>
-    <row r="4" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:71" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>44</v>
+      </c>
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
       <c r="AS4" s="5"/>
     </row>
-    <row r="5" spans="2:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -692,17 +788,72 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-    </row>
-    <row r="6" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="X5" s="31"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="31"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="31"/>
+      <c r="AR5" s="21"/>
+      <c r="AS5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+    </row>
+    <row r="6" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -744,16 +895,67 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AQ6" s="5"/>
-      <c r="AR6" s="5"/>
-      <c r="AS6" s="5"/>
-    </row>
-    <row r="7" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="21"/>
+      <c r="AH6" s="31"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="31"/>
+      <c r="AQ6" s="21"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="1"/>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+    </row>
+    <row r="7" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -796,15 +998,60 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AQ7" s="5"/>
-      <c r="AR7" s="5"/>
-      <c r="AS7" s="5"/>
-    </row>
-    <row r="8" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="31"/>
+      <c r="AR7" s="21"/>
+      <c r="AS7" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="31"/>
+      <c r="AV7" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
+      <c r="BE7" s="1"/>
+      <c r="BF7" s="1"/>
+      <c r="BG7" s="1"/>
+      <c r="BH7" s="1"/>
+      <c r="BI7" s="1"/>
+      <c r="BJ7" s="1"/>
+      <c r="BK7" s="1"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+      <c r="BQ7" s="1"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+    </row>
+    <row r="8" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -848,14 +1095,59 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="5"/>
-      <c r="AS8" s="5"/>
-    </row>
-    <row r="9" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="31"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="31"/>
+      <c r="AS8" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+      <c r="BJ8" s="1"/>
+      <c r="BK8" s="1"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1"/>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+    </row>
+    <row r="9" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -883,12 +1175,55 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AQ9" s="5"/>
-      <c r="AR9" s="5"/>
-      <c r="AS9" s="5"/>
-    </row>
-    <row r="10" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
+      <c r="BJ9" s="1"/>
+      <c r="BK9" s="1"/>
+      <c r="BL9" s="1"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+      <c r="BQ9" s="1"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+    </row>
+    <row r="10" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -917,11 +1252,52 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="5"/>
-      <c r="AS10" s="5"/>
-    </row>
-    <row r="11" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+      <c r="BJ10" s="1"/>
+      <c r="BK10" s="1"/>
+      <c r="BL10" s="1"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+      <c r="BQ10" s="1"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+    </row>
+    <row r="11" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -954,11 +1330,50 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
-      <c r="AQ11" s="5"/>
-      <c r="AR11" s="5"/>
-      <c r="AS11" s="5"/>
-    </row>
-    <row r="12" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BJ11" s="1"/>
+      <c r="BK11" s="1"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
+      <c r="BP11" s="1"/>
+      <c r="BQ11" s="1"/>
+      <c r="BR11" s="1"/>
+      <c r="BS11" s="1"/>
+    </row>
+    <row r="12" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -987,11 +1402,50 @@
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="5"/>
-      <c r="AS12" s="5"/>
-    </row>
-    <row r="13" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="1"/>
+      <c r="BG12" s="1"/>
+      <c r="BH12" s="1"/>
+      <c r="BI12" s="1"/>
+      <c r="BJ12" s="1"/>
+      <c r="BK12" s="1"/>
+      <c r="BL12" s="1"/>
+      <c r="BM12" s="1"/>
+      <c r="BN12" s="1"/>
+      <c r="BO12" s="1"/>
+      <c r="BP12" s="1"/>
+      <c r="BQ12" s="1"/>
+      <c r="BR12" s="1"/>
+      <c r="BS12" s="1"/>
+    </row>
+    <row r="13" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1013,20 +1467,91 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
+      <c r="U13" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="5"/>
-      <c r="AS13" s="5"/>
-    </row>
-    <row r="14" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="Z13" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="15"/>
+      <c r="AT13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="20"/>
+      <c r="AV13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="32"/>
+      <c r="AX13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="35"/>
+      <c r="AZ13" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="38"/>
+      <c r="BB13" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1"/>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1"/>
+      <c r="BJ13" s="1"/>
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="1"/>
+      <c r="BP13" s="1"/>
+      <c r="BQ13" s="1"/>
+      <c r="BR13" s="1"/>
+      <c r="BS13" s="1"/>
+    </row>
+    <row r="14" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1048,20 +1573,73 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
+      <c r="U14" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AQ14" s="5"/>
-      <c r="AR14" s="5"/>
-      <c r="AS14" s="5"/>
-    </row>
-    <row r="15" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="Z14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="19"/>
+      <c r="AT14" s="18"/>
+      <c r="AU14" s="20"/>
+      <c r="AV14" s="21"/>
+      <c r="AW14" s="31"/>
+      <c r="AX14" s="32"/>
+      <c r="AY14" s="34"/>
+      <c r="AZ14" s="33"/>
+      <c r="BA14" s="35"/>
+      <c r="BB14" s="36"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="1"/>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="1"/>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+      <c r="BO14" s="1"/>
+      <c r="BP14" s="1"/>
+      <c r="BQ14" s="1"/>
+      <c r="BR14" s="1"/>
+      <c r="BS14" s="1"/>
+    </row>
+    <row r="15" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1094,11 +1672,50 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-      <c r="AQ15" s="5"/>
-      <c r="AR15" s="5"/>
-      <c r="AS15" s="5"/>
-    </row>
-    <row r="16" spans="2:45" x14ac:dyDescent="0.3">
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+      <c r="BP15" s="1"/>
+      <c r="BQ15" s="1"/>
+      <c r="BR15" s="1"/>
+      <c r="BS15" s="1"/>
+    </row>
+    <row r="16" spans="2:71" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1120,18 +1737,89 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
+      <c r="U16" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AQ16" s="5"/>
-      <c r="AR16" s="5"/>
-      <c r="AS16" s="5"/>
+      <c r="Z16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="20"/>
+      <c r="AV16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="32"/>
+      <c r="AX16" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="33"/>
+      <c r="AZ16" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="36"/>
+      <c r="BB16" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
+      <c r="BJ16" s="1"/>
+      <c r="BK16" s="1"/>
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+      <c r="BP16" s="1"/>
+      <c r="BQ16" s="1"/>
+      <c r="BR16" s="1"/>
+      <c r="BS16" s="1"/>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
@@ -1160,13 +1848,62 @@
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AQ17" s="5"/>
-      <c r="AR17" s="5"/>
-      <c r="AS17" s="5"/>
+      <c r="Z17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="21"/>
+      <c r="AF17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="19"/>
+      <c r="AT17" s="18"/>
+      <c r="AU17" s="20"/>
+      <c r="AV17" s="21"/>
+      <c r="AW17" s="31"/>
+      <c r="AX17" s="32"/>
+      <c r="AY17" s="34"/>
+      <c r="AZ17" s="33"/>
+      <c r="BA17" s="35"/>
+      <c r="BB17" s="36"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+      <c r="BP17" s="1"/>
+      <c r="BQ17" s="1"/>
+      <c r="BR17" s="1"/>
+      <c r="BS17" s="1"/>
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
@@ -1197,9 +1934,48 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-      <c r="AQ18" s="5"/>
-      <c r="AR18" s="5"/>
-      <c r="AS18" s="5"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1"/>
+      <c r="BD18" s="1"/>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="1"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="1"/>
+      <c r="BI18" s="1"/>
+      <c r="BJ18" s="1"/>
+      <c r="BK18" s="1"/>
+      <c r="BL18" s="1"/>
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+      <c r="BO18" s="1"/>
+      <c r="BP18" s="1"/>
+      <c r="BQ18" s="1"/>
+      <c r="BR18" s="1"/>
+      <c r="BS18" s="1"/>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
@@ -1232,9 +2008,48 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
-      <c r="AQ19" s="5"/>
-      <c r="AR19" s="5"/>
-      <c r="AS19" s="5"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="1"/>
+      <c r="BI19" s="1"/>
+      <c r="BJ19" s="1"/>
+      <c r="BK19" s="1"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+      <c r="BO19" s="1"/>
+      <c r="BP19" s="1"/>
+      <c r="BQ19" s="1"/>
+      <c r="BR19" s="1"/>
+      <c r="BS19" s="1"/>
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
@@ -1388,7 +2203,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -1404,7 +2219,7 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
@@ -1420,7 +2235,7 @@
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AS22" s="1"/>
       <c r="AT22" s="1"/>
@@ -1435,7 +2250,9 @@
       <c r="BC22" s="1"/>
       <c r="BD22" s="1"/>
       <c r="BE22" s="1"/>
-      <c r="BF22" s="1"/>
+      <c r="BF22" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="BG22" s="1"/>
       <c r="BH22" s="1"/>
       <c r="BI22" s="1"/>
@@ -1449,7 +2266,9 @@
       <c r="BQ22" s="1"/>
       <c r="BR22" s="1"/>
       <c r="BS22" s="1"/>
-      <c r="BT22" s="1"/>
+      <c r="BT22" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="BU22" s="1"/>
       <c r="BV22" s="1"/>
       <c r="BW22" s="1"/>
@@ -1521,32 +2340,32 @@
       <c r="BC23" s="2"/>
       <c r="BD23" s="1"/>
       <c r="BE23" s="1"/>
-      <c r="BF23" s="1"/>
-      <c r="BG23" s="1"/>
-      <c r="BH23" s="1"/>
-      <c r="BI23" s="1"/>
-      <c r="BJ23" s="1"/>
-      <c r="BK23" s="1"/>
-      <c r="BL23" s="1"/>
-      <c r="BM23" s="1"/>
-      <c r="BN23" s="1"/>
-      <c r="BO23" s="1"/>
-      <c r="BP23" s="1"/>
-      <c r="BQ23" s="1"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
+      <c r="BJ23" s="2"/>
+      <c r="BK23" s="2"/>
+      <c r="BL23" s="2"/>
+      <c r="BM23" s="2"/>
+      <c r="BN23" s="2"/>
+      <c r="BO23" s="2"/>
+      <c r="BP23" s="2"/>
+      <c r="BQ23" s="2"/>
       <c r="BR23" s="1"/>
       <c r="BS23" s="1"/>
-      <c r="BT23" s="1"/>
-      <c r="BU23" s="1"/>
-      <c r="BV23" s="1"/>
-      <c r="BW23" s="1"/>
-      <c r="BX23" s="1"/>
-      <c r="BY23" s="1"/>
-      <c r="BZ23" s="1"/>
-      <c r="CA23" s="1"/>
-      <c r="CB23" s="1"/>
-      <c r="CC23" s="1"/>
-      <c r="CD23" s="1"/>
-      <c r="CE23" s="1"/>
+      <c r="BT23" s="2"/>
+      <c r="BU23" s="2"/>
+      <c r="BV23" s="2"/>
+      <c r="BW23" s="2"/>
+      <c r="BX23" s="2"/>
+      <c r="BY23" s="2"/>
+      <c r="BZ23" s="2"/>
+      <c r="CA23" s="2"/>
+      <c r="CB23" s="2"/>
+      <c r="CC23" s="2"/>
+      <c r="CD23" s="2"/>
+      <c r="CE23" s="2"/>
       <c r="CF23" s="1"/>
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.3">
@@ -1556,7 +2375,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1609,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="AY24" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
@@ -1617,32 +2436,64 @@
       <c r="BC24" s="2"/>
       <c r="BD24" s="1"/>
       <c r="BE24" s="1"/>
-      <c r="BF24" s="1"/>
-      <c r="BG24" s="1"/>
-      <c r="BH24" s="1"/>
-      <c r="BI24" s="1"/>
-      <c r="BJ24" s="1"/>
-      <c r="BK24" s="1"/>
-      <c r="BL24" s="1"/>
-      <c r="BM24" s="1"/>
-      <c r="BN24" s="1"/>
-      <c r="BO24" s="1"/>
-      <c r="BP24" s="1"/>
-      <c r="BQ24" s="1"/>
+      <c r="BF24" s="2"/>
+      <c r="BG24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH24" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ24" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK24" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN24" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO24" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP24" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ24" s="2"/>
       <c r="BR24" s="1"/>
       <c r="BS24" s="1"/>
-      <c r="BT24" s="1"/>
-      <c r="BU24" s="1"/>
-      <c r="BV24" s="1"/>
-      <c r="BW24" s="1"/>
-      <c r="BX24" s="1"/>
-      <c r="BY24" s="1"/>
-      <c r="BZ24" s="1"/>
-      <c r="CA24" s="1"/>
-      <c r="CB24" s="1"/>
-      <c r="CC24" s="1"/>
-      <c r="CD24" s="1"/>
-      <c r="CE24" s="1"/>
+      <c r="BT24" s="2"/>
+      <c r="BU24" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW24" s="20"/>
+      <c r="BX24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BY24" s="32"/>
+      <c r="BZ24" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA24" s="33"/>
+      <c r="CB24" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="CC24" s="36"/>
+      <c r="CD24" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE24" s="2"/>
       <c r="CF24" s="1"/>
     </row>
     <row r="25" spans="1:84" x14ac:dyDescent="0.3">
@@ -1652,7 +2503,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1695,7 +2546,7 @@
       <c r="AS25" s="19"/>
       <c r="AT25" s="18"/>
       <c r="AU25" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AV25" s="20"/>
       <c r="AW25" s="21"/>
@@ -1707,32 +2558,40 @@
       <c r="BC25" s="2"/>
       <c r="BD25" s="1"/>
       <c r="BE25" s="1"/>
-      <c r="BF25" s="1"/>
-      <c r="BG25" s="1"/>
-      <c r="BH25" s="1"/>
-      <c r="BI25" s="1"/>
-      <c r="BJ25" s="1"/>
-      <c r="BK25" s="1"/>
-      <c r="BL25" s="1"/>
-      <c r="BM25" s="1"/>
-      <c r="BN25" s="1"/>
-      <c r="BO25" s="1"/>
-      <c r="BP25" s="1"/>
-      <c r="BQ25" s="1"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="18"/>
+      <c r="BH25" s="20"/>
+      <c r="BI25" s="18"/>
+      <c r="BJ25" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK25" s="20"/>
+      <c r="BL25" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM25" s="21"/>
+      <c r="BN25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO25" s="31"/>
+      <c r="BP25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ25" s="2"/>
       <c r="BR25" s="1"/>
       <c r="BS25" s="1"/>
-      <c r="BT25" s="1"/>
-      <c r="BU25" s="1"/>
-      <c r="BV25" s="1"/>
-      <c r="BW25" s="1"/>
-      <c r="BX25" s="1"/>
-      <c r="BY25" s="1"/>
-      <c r="BZ25" s="1"/>
-      <c r="CA25" s="1"/>
-      <c r="CB25" s="1"/>
-      <c r="CC25" s="1"/>
-      <c r="CD25" s="1"/>
-      <c r="CE25" s="1"/>
+      <c r="BT25" s="2"/>
+      <c r="BU25" s="19"/>
+      <c r="BV25" s="18"/>
+      <c r="BW25" s="20"/>
+      <c r="BX25" s="21"/>
+      <c r="BY25" s="31"/>
+      <c r="BZ25" s="32"/>
+      <c r="CA25" s="34"/>
+      <c r="CB25" s="33"/>
+      <c r="CC25" s="35"/>
+      <c r="CD25" s="36"/>
+      <c r="CE25" s="2"/>
       <c r="CF25" s="1"/>
     </row>
     <row r="26" spans="1:84" x14ac:dyDescent="0.3">
@@ -1741,7 +2600,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
@@ -1797,32 +2656,32 @@
       <c r="BC26" s="2"/>
       <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
-      <c r="BF26" s="1"/>
-      <c r="BG26" s="1"/>
-      <c r="BH26" s="1"/>
-      <c r="BI26" s="1"/>
-      <c r="BJ26" s="1"/>
-      <c r="BK26" s="1"/>
-      <c r="BL26" s="1"/>
-      <c r="BM26" s="1"/>
-      <c r="BN26" s="1"/>
-      <c r="BO26" s="1"/>
-      <c r="BP26" s="1"/>
-      <c r="BQ26" s="1"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="20"/>
+      <c r="BH26" s="21"/>
+      <c r="BI26" s="20"/>
+      <c r="BJ26" s="20"/>
+      <c r="BK26" s="21"/>
+      <c r="BL26" s="21"/>
+      <c r="BM26" s="31"/>
+      <c r="BN26" s="31"/>
+      <c r="BO26" s="32"/>
+      <c r="BP26" s="32"/>
+      <c r="BQ26" s="2"/>
       <c r="BR26" s="1"/>
       <c r="BS26" s="1"/>
-      <c r="BT26" s="1"/>
-      <c r="BU26" s="1"/>
-      <c r="BV26" s="1"/>
-      <c r="BW26" s="1"/>
-      <c r="BX26" s="1"/>
-      <c r="BY26" s="1"/>
-      <c r="BZ26" s="1"/>
-      <c r="CA26" s="1"/>
-      <c r="CB26" s="1"/>
-      <c r="CC26" s="1"/>
-      <c r="CD26" s="1"/>
-      <c r="CE26" s="1"/>
+      <c r="BT26" s="2"/>
+      <c r="BU26" s="18"/>
+      <c r="BV26" s="20"/>
+      <c r="BW26" s="21"/>
+      <c r="BX26" s="31"/>
+      <c r="BY26" s="32"/>
+      <c r="BZ26" s="34"/>
+      <c r="CA26" s="33"/>
+      <c r="CB26" s="35"/>
+      <c r="CC26" s="36"/>
+      <c r="CD26" s="37"/>
+      <c r="CE26" s="2"/>
       <c r="CF26" s="1"/>
     </row>
     <row r="27" spans="1:84" x14ac:dyDescent="0.3">
@@ -1833,7 +2692,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
       <c r="G27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1873,7 +2732,7 @@
       <c r="AQ27" s="1"/>
       <c r="AR27" s="2"/>
       <c r="AS27" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AT27" s="20"/>
       <c r="AU27" s="21"/>
@@ -1889,32 +2748,38 @@
       <c r="BC27" s="2"/>
       <c r="BD27" s="1"/>
       <c r="BE27" s="1"/>
-      <c r="BF27" s="1"/>
-      <c r="BG27" s="1"/>
-      <c r="BH27" s="1"/>
-      <c r="BI27" s="1"/>
-      <c r="BJ27" s="1"/>
-      <c r="BK27" s="1"/>
-      <c r="BL27" s="1"/>
-      <c r="BM27" s="1"/>
-      <c r="BN27" s="1"/>
-      <c r="BO27" s="1"/>
-      <c r="BP27" s="1"/>
-      <c r="BQ27" s="1"/>
+      <c r="BF27" s="2"/>
+      <c r="BG27" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH27" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI27" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ27" s="21"/>
+      <c r="BK27" s="31"/>
+      <c r="BL27" s="31"/>
+      <c r="BM27" s="32"/>
+      <c r="BN27" s="32"/>
+      <c r="BO27" s="34"/>
+      <c r="BP27" s="34"/>
+      <c r="BQ27" s="2"/>
       <c r="BR27" s="1"/>
       <c r="BS27" s="1"/>
-      <c r="BT27" s="1"/>
-      <c r="BU27" s="1"/>
-      <c r="BV27" s="1"/>
-      <c r="BW27" s="1"/>
-      <c r="BX27" s="1"/>
-      <c r="BY27" s="1"/>
-      <c r="BZ27" s="1"/>
-      <c r="CA27" s="1"/>
-      <c r="CB27" s="1"/>
-      <c r="CC27" s="1"/>
+      <c r="BT27" s="2"/>
+      <c r="BU27" s="20"/>
+      <c r="BV27" s="21"/>
+      <c r="BW27" s="31"/>
+      <c r="BX27" s="32"/>
+      <c r="BY27" s="34"/>
+      <c r="BZ27" s="33"/>
+      <c r="CA27" s="35"/>
+      <c r="CB27" s="36"/>
+      <c r="CC27" s="37"/>
       <c r="CD27" s="1"/>
-      <c r="CE27" s="1"/>
+      <c r="CE27" s="2"/>
       <c r="CF27" s="1"/>
     </row>
     <row r="28" spans="1:84" x14ac:dyDescent="0.3">
@@ -1925,14 +2790,14 @@
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
       <c r="G28" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1950,7 +2815,7 @@
         <v>2</v>
       </c>
       <c r="V28" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>0</v>
@@ -1966,10 +2831,10 @@
       <c r="AF28" s="23"/>
       <c r="AG28" s="23"/>
       <c r="AH28" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AI28" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AJ28" s="23" t="s">
         <v>2</v>
@@ -1988,13 +2853,13 @@
         <v>0</v>
       </c>
       <c r="AT28" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AU28" s="20" t="s">
         <v>0</v>
       </c>
       <c r="AV28" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
@@ -2005,56 +2870,62 @@
       <c r="BC28" s="2"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1"/>
-      <c r="BF28" s="1"/>
-      <c r="BG28" s="1"/>
-      <c r="BH28" s="1"/>
-      <c r="BI28" s="1"/>
-      <c r="BJ28" s="1"/>
-      <c r="BK28" s="1"/>
-      <c r="BL28" s="1"/>
-      <c r="BM28" s="1"/>
-      <c r="BN28" s="1"/>
+      <c r="BF28" s="2"/>
+      <c r="BG28" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH28" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI28" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ28" s="31"/>
+      <c r="BK28" s="32"/>
+      <c r="BL28" s="32"/>
+      <c r="BM28" s="34"/>
+      <c r="BN28" s="34"/>
       <c r="BO28" s="1"/>
       <c r="BP28" s="1"/>
-      <c r="BQ28" s="1"/>
+      <c r="BQ28" s="2"/>
       <c r="BR28" s="1"/>
       <c r="BS28" s="1"/>
-      <c r="BT28" s="1"/>
-      <c r="BU28" s="1"/>
-      <c r="BV28" s="1"/>
-      <c r="BW28" s="1"/>
-      <c r="BX28" s="1"/>
-      <c r="BY28" s="1"/>
-      <c r="BZ28" s="1"/>
-      <c r="CA28" s="1"/>
-      <c r="CB28" s="1"/>
+      <c r="BT28" s="2"/>
+      <c r="BU28" s="21"/>
+      <c r="BV28" s="31"/>
+      <c r="BW28" s="32"/>
+      <c r="BX28" s="34"/>
+      <c r="BY28" s="33"/>
+      <c r="BZ28" s="35"/>
+      <c r="CA28" s="36"/>
+      <c r="CB28" s="37"/>
       <c r="CC28" s="1"/>
       <c r="CD28" s="1"/>
-      <c r="CE28" s="1"/>
+      <c r="CE28" s="2"/>
       <c r="CF28" s="1"/>
     </row>
     <row r="29" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="4"/>
       <c r="J29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -2067,13 +2938,13 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V29" s="4"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z29" s="1"/>
       <c r="AA29" s="2"/>
@@ -2084,7 +2955,7 @@
       <c r="AF29" s="23"/>
       <c r="AG29" s="23"/>
       <c r="AH29" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AI29" s="23"/>
       <c r="AJ29" s="23" t="s">
@@ -2115,32 +2986,32 @@
       <c r="BC29" s="2"/>
       <c r="BD29" s="1"/>
       <c r="BE29" s="1"/>
-      <c r="BF29" s="1"/>
-      <c r="BG29" s="1"/>
-      <c r="BH29" s="1"/>
-      <c r="BI29" s="1"/>
-      <c r="BJ29" s="1"/>
-      <c r="BK29" s="1"/>
-      <c r="BL29" s="1"/>
+      <c r="BF29" s="2"/>
+      <c r="BG29" s="32"/>
+      <c r="BH29" s="34"/>
+      <c r="BI29" s="32"/>
+      <c r="BJ29" s="32"/>
+      <c r="BK29" s="34"/>
+      <c r="BL29" s="34"/>
       <c r="BM29" s="1"/>
       <c r="BN29" s="1"/>
       <c r="BO29" s="1"/>
       <c r="BP29" s="1"/>
-      <c r="BQ29" s="1"/>
+      <c r="BQ29" s="2"/>
       <c r="BR29" s="1"/>
       <c r="BS29" s="1"/>
-      <c r="BT29" s="1"/>
-      <c r="BU29" s="1"/>
-      <c r="BV29" s="1"/>
-      <c r="BW29" s="1"/>
-      <c r="BX29" s="1"/>
-      <c r="BY29" s="1"/>
-      <c r="BZ29" s="1"/>
-      <c r="CA29" s="1"/>
+      <c r="BT29" s="2"/>
+      <c r="BU29" s="31"/>
+      <c r="BV29" s="32"/>
+      <c r="BW29" s="34"/>
+      <c r="BX29" s="33"/>
+      <c r="BY29" s="35"/>
+      <c r="BZ29" s="36"/>
+      <c r="CA29" s="37"/>
       <c r="CB29" s="1"/>
       <c r="CC29" s="1"/>
       <c r="CD29" s="1"/>
-      <c r="CE29" s="1"/>
+      <c r="CE29" s="2"/>
       <c r="CF29" s="1"/>
     </row>
     <row r="30" spans="1:84" x14ac:dyDescent="0.3">
@@ -2153,7 +3024,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="4"/>
       <c r="I30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2173,10 +3044,10 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AA30" s="2"/>
       <c r="AB30" s="1"/>
@@ -2193,7 +3064,7 @@
         <v>2</v>
       </c>
       <c r="AK30" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AL30" s="22"/>
       <c r="AM30" s="23"/>
@@ -2217,32 +3088,32 @@
       <c r="BC30" s="2"/>
       <c r="BD30" s="1"/>
       <c r="BE30" s="1"/>
-      <c r="BF30" s="1"/>
-      <c r="BG30" s="1"/>
+      <c r="BF30" s="2"/>
+      <c r="BG30" s="34"/>
       <c r="BH30" s="1"/>
-      <c r="BI30" s="1"/>
-      <c r="BJ30" s="1"/>
+      <c r="BI30" s="34"/>
+      <c r="BJ30" s="34"/>
       <c r="BK30" s="1"/>
       <c r="BL30" s="1"/>
       <c r="BM30" s="1"/>
       <c r="BN30" s="1"/>
       <c r="BO30" s="1"/>
       <c r="BP30" s="1"/>
-      <c r="BQ30" s="1"/>
+      <c r="BQ30" s="2"/>
       <c r="BR30" s="1"/>
       <c r="BS30" s="1"/>
-      <c r="BT30" s="1"/>
-      <c r="BU30" s="1"/>
-      <c r="BV30" s="1"/>
-      <c r="BW30" s="1"/>
-      <c r="BX30" s="1"/>
-      <c r="BY30" s="1"/>
-      <c r="BZ30" s="1"/>
+      <c r="BT30" s="2"/>
+      <c r="BU30" s="32"/>
+      <c r="BV30" s="34"/>
+      <c r="BW30" s="33"/>
+      <c r="BX30" s="35"/>
+      <c r="BY30" s="36"/>
+      <c r="BZ30" s="37"/>
       <c r="CA30" s="1"/>
       <c r="CB30" s="1"/>
       <c r="CC30" s="1"/>
       <c r="CD30" s="1"/>
-      <c r="CE30" s="1"/>
+      <c r="CE30" s="2"/>
       <c r="CF30" s="1"/>
     </row>
     <row r="31" spans="1:84" x14ac:dyDescent="0.3">
@@ -2250,26 +3121,26 @@
       <c r="B31" s="2"/>
       <c r="C31" s="4"/>
       <c r="D31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="2"/>
@@ -2283,13 +3154,13 @@
       <c r="U31" s="3"/>
       <c r="V31" s="4"/>
       <c r="W31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y31" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>0</v>
@@ -2306,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="AJ31" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AK31" s="6"/>
       <c r="AL31" s="22"/>
@@ -2333,7 +3204,7 @@
       <c r="BC31" s="2"/>
       <c r="BD31" s="1"/>
       <c r="BE31" s="1"/>
-      <c r="BF31" s="1"/>
+      <c r="BF31" s="2"/>
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
       <c r="BI31" s="1"/>
@@ -2344,21 +3215,21 @@
       <c r="BN31" s="1"/>
       <c r="BO31" s="1"/>
       <c r="BP31" s="1"/>
-      <c r="BQ31" s="1"/>
+      <c r="BQ31" s="2"/>
       <c r="BR31" s="1"/>
       <c r="BS31" s="1"/>
-      <c r="BT31" s="1"/>
-      <c r="BU31" s="1"/>
-      <c r="BV31" s="1"/>
-      <c r="BW31" s="1"/>
-      <c r="BX31" s="1"/>
-      <c r="BY31" s="1"/>
+      <c r="BT31" s="2"/>
+      <c r="BU31" s="34"/>
+      <c r="BV31" s="33"/>
+      <c r="BW31" s="35"/>
+      <c r="BX31" s="36"/>
+      <c r="BY31" s="37"/>
       <c r="BZ31" s="1"/>
       <c r="CA31" s="1"/>
       <c r="CB31" s="1"/>
       <c r="CC31" s="1"/>
       <c r="CD31" s="1"/>
-      <c r="CE31" s="1"/>
+      <c r="CE31" s="2"/>
       <c r="CF31" s="1"/>
     </row>
     <row r="32" spans="1:84" x14ac:dyDescent="0.3">
@@ -2366,7 +3237,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="4"/>
       <c r="D32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2376,7 +3247,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="15"/>
       <c r="L32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="1"/>
@@ -2388,11 +3259,11 @@
       <c r="T32" s="1"/>
       <c r="U32" s="4"/>
       <c r="V32" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W32" s="4"/>
       <c r="X32" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y32" s="25"/>
       <c r="Z32" s="1" t="s">
@@ -2414,7 +3285,7 @@
       </c>
       <c r="AK32" s="22"/>
       <c r="AL32" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AM32" s="23" t="s">
         <v>2</v>
@@ -2441,7 +3312,7 @@
       <c r="BC32" s="2"/>
       <c r="BD32" s="1"/>
       <c r="BE32" s="1"/>
-      <c r="BF32" s="1"/>
+      <c r="BF32" s="2"/>
       <c r="BG32" s="1"/>
       <c r="BH32" s="1"/>
       <c r="BI32" s="1"/>
@@ -2452,21 +3323,23 @@
       <c r="BN32" s="1"/>
       <c r="BO32" s="1"/>
       <c r="BP32" s="1"/>
-      <c r="BQ32" s="1"/>
+      <c r="BQ32" s="2"/>
       <c r="BR32" s="1"/>
       <c r="BS32" s="1"/>
-      <c r="BT32" s="1"/>
-      <c r="BU32" s="1"/>
-      <c r="BV32" s="1"/>
-      <c r="BW32" s="1"/>
-      <c r="BX32" s="1"/>
+      <c r="BT32" s="2"/>
+      <c r="BU32" s="33"/>
+      <c r="BV32" s="35"/>
+      <c r="BW32" s="36"/>
+      <c r="BX32" s="37"/>
       <c r="BY32" s="1"/>
       <c r="BZ32" s="1"/>
       <c r="CA32" s="1"/>
       <c r="CB32" s="1"/>
       <c r="CC32" s="1"/>
-      <c r="CD32" s="1"/>
-      <c r="CE32" s="1"/>
+      <c r="CD32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE32" s="2"/>
       <c r="CF32" s="1"/>
     </row>
     <row r="33" spans="1:84" x14ac:dyDescent="0.3">
@@ -2481,10 +3354,10 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="1"/>
@@ -2495,7 +3368,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>0</v>
@@ -2547,7 +3420,7 @@
       <c r="BC33" s="2"/>
       <c r="BD33" s="1"/>
       <c r="BE33" s="1"/>
-      <c r="BF33" s="1"/>
+      <c r="BF33" s="2"/>
       <c r="BG33" s="1"/>
       <c r="BH33" s="1"/>
       <c r="BI33" s="1"/>
@@ -2558,21 +3431,25 @@
       <c r="BN33" s="1"/>
       <c r="BO33" s="1"/>
       <c r="BP33" s="1"/>
-      <c r="BQ33" s="1"/>
+      <c r="BQ33" s="2"/>
       <c r="BR33" s="1"/>
       <c r="BS33" s="1"/>
-      <c r="BT33" s="1"/>
-      <c r="BU33" s="1"/>
-      <c r="BV33" s="1"/>
-      <c r="BW33" s="1"/>
+      <c r="BT33" s="2"/>
+      <c r="BU33" s="35"/>
+      <c r="BV33" s="36"/>
+      <c r="BW33" s="37"/>
       <c r="BX33" s="1"/>
       <c r="BY33" s="1"/>
       <c r="BZ33" s="1"/>
       <c r="CA33" s="1"/>
       <c r="CB33" s="1"/>
-      <c r="CC33" s="1"/>
-      <c r="CD33" s="1"/>
-      <c r="CE33" s="1"/>
+      <c r="CC33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE33" s="2"/>
       <c r="CF33" s="1"/>
     </row>
     <row r="34" spans="1:84" x14ac:dyDescent="0.3">
@@ -2633,32 +3510,32 @@
       <c r="BC34" s="2"/>
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
-      <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
-      <c r="BH34" s="1"/>
-      <c r="BI34" s="1"/>
-      <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
-      <c r="BL34" s="1"/>
-      <c r="BM34" s="1"/>
-      <c r="BN34" s="1"/>
-      <c r="BO34" s="1"/>
-      <c r="BP34" s="1"/>
-      <c r="BQ34" s="1"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34" s="2"/>
+      <c r="BH34" s="2"/>
+      <c r="BI34" s="2"/>
+      <c r="BJ34" s="2"/>
+      <c r="BK34" s="2"/>
+      <c r="BL34" s="2"/>
+      <c r="BM34" s="2"/>
+      <c r="BN34" s="2"/>
+      <c r="BO34" s="2"/>
+      <c r="BP34" s="2"/>
+      <c r="BQ34" s="2"/>
       <c r="BR34" s="1"/>
       <c r="BS34" s="1"/>
-      <c r="BT34" s="1"/>
-      <c r="BU34" s="1"/>
-      <c r="BV34" s="1"/>
-      <c r="BW34" s="1"/>
-      <c r="BX34" s="1"/>
-      <c r="BY34" s="1"/>
-      <c r="BZ34" s="1"/>
-      <c r="CA34" s="1"/>
-      <c r="CB34" s="1"/>
-      <c r="CC34" s="1"/>
-      <c r="CD34" s="1"/>
-      <c r="CE34" s="1"/>
+      <c r="BT34" s="2"/>
+      <c r="BU34" s="2"/>
+      <c r="BV34" s="2"/>
+      <c r="BW34" s="2"/>
+      <c r="BX34" s="2"/>
+      <c r="BY34" s="2"/>
+      <c r="BZ34" s="2"/>
+      <c r="CA34" s="2"/>
+      <c r="CB34" s="2"/>
+      <c r="CC34" s="2"/>
+      <c r="CD34" s="2"/>
+      <c r="CE34" s="2"/>
       <c r="CF34" s="1"/>
     </row>
     <row r="35" spans="1:84" x14ac:dyDescent="0.3">
@@ -4039,7 +4916,7 @@
     </row>
     <row r="51" spans="1:84" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>

</xml_diff>